<commit_message>
Added 4 studies to dataset and model: 4007, 4000, 3843, 3875
</commit_message>
<xml_diff>
--- a/IH_effectiveness_data_Extraction_comparative studies_revised_03242015.xlsx
+++ b/IH_effectiveness_data_Extraction_comparative studies_revised_03242015.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25711"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fonnescj/Dropbox/Collaborations/Infantile Hemangioma/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fonnescj/GitHub/IH_meta-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="14080" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1760" yWindow="1800" windowWidth="20480" windowHeight="14080" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KQ2_study characteristics" sheetId="3" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5254" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5462" uniqueCount="550">
   <si>
     <t>PMID</t>
   </si>
@@ -1734,12 +1734,145 @@
   <si>
     <t>none</t>
   </si>
+  <si>
+    <t>Double-blind randomized pilot trial evaluating the efficacy of oral propranolol on infantile haemangiomas in infants &lt; 4 months of age</t>
+  </si>
+  <si>
+    <t>3 then 4</t>
+  </si>
+  <si>
+    <t>Effect of propranolol vs prednisolone vs propranolol with prednisolone in the management of infantile hemangioma: a randomized controlled study</t>
+  </si>
+  <si>
+    <t>Malik</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>Topical Timolol Solution Versus Laser in
+Treatment of Infantile Hemangioma:
+A Comparative Study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg/ml </t>
+  </si>
+  <si>
+    <t>Topical timolol maleate 0.5% for infantile hemangioma;
+it’s effectiveness and/or adjunctive pulsed dye laser – single center
+experience of 102 cases in Korea</t>
+  </si>
+  <si>
+    <t>Park</t>
+  </si>
+  <si>
+    <t>change in thickness</t>
+  </si>
+  <si>
+    <t>percentage change in size</t>
+  </si>
+  <si>
+    <t>color fading, flattening</t>
+  </si>
+  <si>
+    <t>mean size reduction</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">No improvement (0 %) in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 6month old</t>
+    </r>
+  </si>
+  <si>
+    <t>Mild improvement (&lt;25%) in ≤ 6month old</t>
+  </si>
+  <si>
+    <t>Moderate imrovement (26% - 50%) in ≤ 6month old</t>
+  </si>
+  <si>
+    <t>Good improvement (51% - 75%) in ≤ 6month old</t>
+  </si>
+  <si>
+    <t>Excellent improvement (76% 110%)  in ≤ 6month old</t>
+  </si>
+  <si>
+    <t>No improvement (0 %) in &gt; 6month old</t>
+  </si>
+  <si>
+    <t>Mild improvement (&lt;25%) in &gt; 6month old</t>
+  </si>
+  <si>
+    <t>Moderate imrovement (26% - 50%) in &gt; 6month old</t>
+  </si>
+  <si>
+    <t>Good improvement (51% - 75%) in &gt; 6month old</t>
+  </si>
+  <si>
+    <t>Excellent improvement (76% 110%)  in &gt; 6month old</t>
+  </si>
+  <si>
+    <t>Hemoglobin level after treatment</t>
+  </si>
+  <si>
+    <t>Improvement &lt; 0</t>
+  </si>
+  <si>
+    <t>Improvement = 0</t>
+  </si>
+  <si>
+    <t>Improvement = 0 - 24</t>
+  </si>
+  <si>
+    <t>Improvement = 25 - 49</t>
+  </si>
+  <si>
+    <t>Improvement = 50 - 74</t>
+  </si>
+  <si>
+    <t>Improvement = 75 - 100</t>
+  </si>
+  <si>
+    <t>3 months post Rx</t>
+  </si>
+  <si>
+    <t>3 and 6 months from Rx initiation</t>
+  </si>
+  <si>
+    <t>44.9 (36.0, 76.2)</t>
+  </si>
+  <si>
+    <t>15.8 (2.4, 51.7)</t>
+  </si>
+  <si>
+    <t>89.8 ± 10.3</t>
+  </si>
+  <si>
+    <t>66.6 ± 41.6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1835,8 +1968,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1882,12 +2021,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1942,7 +2075,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2079,15 +2212,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -2097,8 +2221,23 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="39">
@@ -12069,34 +12208,38 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:W84"/>
+  <dimension ref="A1:W109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" style="11" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="0.1640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" style="11" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="11" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="6.5" style="11" customWidth="1"/>
-    <col min="12" max="12" width="8" style="11" customWidth="1"/>
-    <col min="13" max="13" width="43.6640625" style="11" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" style="13" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5" style="13" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5" customWidth="1"/>
-    <col min="17" max="20" width="17.5" style="53" customWidth="1"/>
-    <col min="21" max="22" width="11" style="13"/>
-    <col min="23" max="16384" width="11" style="11"/>
+    <col min="1" max="1" width="5.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="102" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5" style="50" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10" style="50" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="11" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="14" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12139,25 +12282,25 @@
       <c r="M1" s="14" t="s">
         <v>490</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="N1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="14" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="14" t="s">
         <v>492</v>
       </c>
-      <c r="Q1" s="51" t="s">
+      <c r="Q1" s="48" t="s">
         <v>494</v>
       </c>
-      <c r="R1" s="51" t="s">
+      <c r="R1" s="48" t="s">
         <v>502</v>
       </c>
-      <c r="S1" s="51" t="s">
+      <c r="S1" s="48" t="s">
         <v>495</v>
       </c>
-      <c r="T1" s="51" t="s">
+      <c r="T1" s="48" t="s">
         <v>496</v>
       </c>
       <c r="U1" s="14" t="s">
@@ -12204,21 +12347,21 @@
       <c r="M2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="49" t="s">
+      <c r="N2" s="11" t="s">
         <v>463</v>
       </c>
-      <c r="O2" s="49" t="s">
+      <c r="O2" s="11" t="s">
         <v>20</v>
       </c>
       <c r="P2" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52">
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49">
         <v>99</v>
       </c>
-      <c r="T2" s="52">
+      <c r="T2" s="49">
         <v>100</v>
       </c>
       <c r="U2" s="11">
@@ -12265,21 +12408,21 @@
       <c r="M3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="49" t="s">
+      <c r="N3" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="O3" s="49" t="s">
+      <c r="O3" s="11" t="s">
         <v>20</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52">
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49">
         <v>99</v>
       </c>
-      <c r="T3" s="52">
+      <c r="T3" s="49">
         <v>100</v>
       </c>
       <c r="U3" s="11">
@@ -12326,21 +12469,21 @@
       <c r="M4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="49" t="s">
+      <c r="N4" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="O4" s="49" t="s">
+      <c r="O4" s="11" t="s">
         <v>20</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="Q4" s="52"/>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52">
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49">
         <v>1</v>
       </c>
-      <c r="T4" s="52">
+      <c r="T4" s="49">
         <v>99</v>
       </c>
       <c r="U4" s="11">
@@ -12387,19 +12530,19 @@
       <c r="M5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="49" t="s">
+      <c r="N5" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="O5" s="49" t="s">
+      <c r="O5" s="11" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S5" s="53">
+      <c r="S5" s="50">
         <v>1</v>
       </c>
-      <c r="T5" s="53">
+      <c r="T5" s="50">
         <v>99</v>
       </c>
       <c r="U5" s="11">
@@ -12448,19 +12591,19 @@
       <c r="M6" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="N6" s="50">
+      <c r="N6" s="13">
         <v>60</v>
       </c>
-      <c r="O6" s="50" t="s">
+      <c r="O6" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S6" s="53">
+      <c r="S6" s="50">
         <v>5</v>
       </c>
-      <c r="T6" s="53">
+      <c r="T6" s="50">
         <v>100</v>
       </c>
       <c r="U6" s="13">
@@ -12510,19 +12653,19 @@
       <c r="M7" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="N7" s="50">
+      <c r="N7" s="13">
         <v>11</v>
       </c>
-      <c r="O7" s="50" t="s">
+      <c r="O7" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P7" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S7" s="53">
+      <c r="S7" s="50">
         <v>5</v>
       </c>
-      <c r="T7" s="53">
+      <c r="T7" s="50">
         <v>100</v>
       </c>
       <c r="U7" s="13">
@@ -12570,19 +12713,19 @@
       <c r="M8" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="N8" s="50" t="s">
+      <c r="N8" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="O8" s="50" t="s">
+      <c r="O8" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P8" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S8" s="53">
+      <c r="S8" s="50">
         <v>50</v>
       </c>
-      <c r="T8" s="53">
+      <c r="T8" s="50">
         <v>100</v>
       </c>
       <c r="U8" s="13">
@@ -12629,19 +12772,19 @@
       <c r="M9" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="N9" s="50" t="s">
+      <c r="N9" s="13" t="s">
         <v>468</v>
       </c>
-      <c r="O9" s="50" t="s">
+      <c r="O9" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P9" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S9" s="53">
+      <c r="S9" s="50">
         <v>50</v>
       </c>
-      <c r="T9" s="53">
+      <c r="T9" s="50">
         <v>100</v>
       </c>
       <c r="U9" s="13">
@@ -12688,19 +12831,19 @@
       <c r="M10" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="N10" s="50">
+      <c r="N10" s="13">
         <v>0</v>
       </c>
-      <c r="O10" s="50" t="s">
+      <c r="O10" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P10" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S10" s="53">
+      <c r="S10" s="50">
         <v>50</v>
       </c>
-      <c r="T10" s="53">
+      <c r="T10" s="50">
         <v>100</v>
       </c>
       <c r="U10" s="13">
@@ -12747,19 +12890,19 @@
       <c r="M11" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="N11" s="50" t="s">
+      <c r="N11" s="13" t="s">
         <v>468</v>
       </c>
-      <c r="O11" s="50" t="s">
+      <c r="O11" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P11" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S11" s="53">
+      <c r="S11" s="50">
         <v>10</v>
       </c>
-      <c r="T11" s="53">
+      <c r="T11" s="50">
         <v>50</v>
       </c>
       <c r="U11" s="13">
@@ -12806,19 +12949,19 @@
       <c r="M12" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="N12" s="50" t="s">
+      <c r="N12" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="O12" s="50" t="s">
+      <c r="O12" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P12" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S12" s="53">
+      <c r="S12" s="50">
         <v>10</v>
       </c>
-      <c r="T12" s="53">
+      <c r="T12" s="50">
         <v>50</v>
       </c>
       <c r="U12" s="13">
@@ -12865,19 +13008,19 @@
       <c r="M13" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="N13" s="50" t="s">
+      <c r="N13" s="13" t="s">
         <v>469</v>
       </c>
-      <c r="O13" s="50" t="s">
+      <c r="O13" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P13" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S13" s="53">
+      <c r="S13" s="50">
         <v>10</v>
       </c>
-      <c r="T13" s="53">
+      <c r="T13" s="50">
         <v>50</v>
       </c>
       <c r="U13" s="13">
@@ -12924,19 +13067,19 @@
       <c r="M14" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="N14" s="50" t="s">
+      <c r="N14" s="13" t="s">
         <v>470</v>
       </c>
-      <c r="O14" s="50" t="s">
+      <c r="O14" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P14" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S14" s="53">
+      <c r="S14" s="50">
         <v>0</v>
       </c>
-      <c r="T14" s="53">
+      <c r="T14" s="50">
         <v>10</v>
       </c>
       <c r="U14" s="13">
@@ -12983,19 +13126,19 @@
       <c r="M15" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="N15" s="50" t="s">
+      <c r="N15" s="13" t="s">
         <v>470</v>
       </c>
-      <c r="O15" s="50" t="s">
+      <c r="O15" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S15" s="53">
+      <c r="S15" s="50">
         <v>0</v>
       </c>
-      <c r="T15" s="53">
+      <c r="T15" s="50">
         <v>10</v>
       </c>
       <c r="U15" s="13">
@@ -13042,19 +13185,19 @@
       <c r="M16" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="N16" s="50" t="s">
+      <c r="N16" s="13" t="s">
         <v>471</v>
       </c>
-      <c r="O16" s="50" t="s">
+      <c r="O16" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S16" s="53">
+      <c r="S16" s="50">
         <v>0</v>
       </c>
-      <c r="T16" s="53">
+      <c r="T16" s="50">
         <v>10</v>
       </c>
       <c r="U16" s="13">
@@ -13101,19 +13244,19 @@
       <c r="M17" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="N17" s="50" t="s">
+      <c r="N17" s="13" t="s">
         <v>472</v>
       </c>
-      <c r="O17" s="50" t="s">
+      <c r="O17" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P17" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S17" s="53">
+      <c r="S17" s="50">
         <v>99</v>
       </c>
-      <c r="T17" s="53">
+      <c r="T17" s="50">
         <v>100</v>
       </c>
       <c r="U17" s="13">
@@ -13160,19 +13303,19 @@
       <c r="M18" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="N18" s="50" t="s">
+      <c r="N18" s="13" t="s">
         <v>473</v>
       </c>
-      <c r="O18" s="50" t="s">
+      <c r="O18" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P18" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S18" s="53">
+      <c r="S18" s="50">
         <v>99</v>
       </c>
-      <c r="T18" s="53">
+      <c r="T18" s="50">
         <v>100</v>
       </c>
       <c r="U18" s="13">
@@ -13219,19 +13362,19 @@
       <c r="M19" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="N19" s="50" t="s">
+      <c r="N19" s="13" t="s">
         <v>474</v>
       </c>
-      <c r="O19" s="50" t="s">
+      <c r="O19" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P19" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S19" s="53">
+      <c r="S19" s="50">
         <v>99</v>
       </c>
-      <c r="T19" s="53">
+      <c r="T19" s="50">
         <v>100</v>
       </c>
       <c r="U19" s="13">
@@ -13278,19 +13421,19 @@
       <c r="M20" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="N20" s="50" t="s">
+      <c r="N20" s="13" t="s">
         <v>474</v>
       </c>
-      <c r="O20" s="50" t="s">
+      <c r="O20" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P20" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S20" s="53">
+      <c r="S20" s="50">
         <v>50</v>
       </c>
-      <c r="T20" s="53">
+      <c r="T20" s="50">
         <v>99</v>
       </c>
       <c r="U20" s="13">
@@ -13337,19 +13480,19 @@
       <c r="M21" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="N21" s="50" t="s">
+      <c r="N21" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="O21" s="50" t="s">
+      <c r="O21" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P21" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S21" s="53">
+      <c r="S21" s="50">
         <v>50</v>
       </c>
-      <c r="T21" s="53">
+      <c r="T21" s="50">
         <v>99</v>
       </c>
       <c r="U21" s="13">
@@ -13396,19 +13539,19 @@
       <c r="M22" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="N22" s="50" t="s">
+      <c r="N22" s="13" t="s">
         <v>473</v>
       </c>
-      <c r="O22" s="50" t="s">
+      <c r="O22" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P22" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S22" s="53">
+      <c r="S22" s="50">
         <v>50</v>
       </c>
-      <c r="T22" s="53">
+      <c r="T22" s="50">
         <v>99</v>
       </c>
       <c r="U22" s="13">
@@ -13455,19 +13598,19 @@
       <c r="M23" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="N23" s="50" t="s">
+      <c r="N23" s="13" t="s">
         <v>476</v>
       </c>
-      <c r="O23" s="50" t="s">
+      <c r="O23" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P23" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S23" s="53">
+      <c r="S23" s="50">
         <v>1</v>
       </c>
-      <c r="T23" s="53">
+      <c r="T23" s="50">
         <v>50</v>
       </c>
       <c r="U23" s="13">
@@ -13514,19 +13657,19 @@
       <c r="M24" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="N24" s="50" t="s">
+      <c r="N24" s="13" t="s">
         <v>474</v>
       </c>
-      <c r="O24" s="50" t="s">
+      <c r="O24" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P24" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S24" s="53">
+      <c r="S24" s="50">
         <v>1</v>
       </c>
-      <c r="T24" s="53">
+      <c r="T24" s="50">
         <v>50</v>
       </c>
       <c r="U24" s="13">
@@ -13573,19 +13716,19 @@
       <c r="M25" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="N25" s="50" t="s">
+      <c r="N25" s="13" t="s">
         <v>473</v>
       </c>
-      <c r="O25" s="50" t="s">
+      <c r="O25" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P25" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S25" s="53">
+      <c r="S25" s="50">
         <v>1</v>
       </c>
-      <c r="T25" s="53">
+      <c r="T25" s="50">
         <v>50</v>
       </c>
       <c r="U25" s="13">
@@ -13632,19 +13775,19 @@
       <c r="M26" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="N26" s="50" t="s">
+      <c r="N26" s="13" t="s">
         <v>473</v>
       </c>
-      <c r="O26" s="50" t="s">
+      <c r="O26" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P26" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="S26" s="53">
+      <c r="S26" s="50">
         <v>0</v>
       </c>
-      <c r="T26" s="53">
+      <c r="T26" s="50">
         <v>1</v>
       </c>
       <c r="U26" s="13">
@@ -13691,19 +13834,19 @@
       <c r="M27" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="N27" s="50" t="s">
+      <c r="N27" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="O27" s="50" t="s">
+      <c r="O27" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P27" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="S27" s="53">
+      <c r="S27" s="50">
         <v>0</v>
       </c>
-      <c r="T27" s="53">
+      <c r="T27" s="50">
         <v>1</v>
       </c>
       <c r="U27" s="13">
@@ -13750,19 +13893,19 @@
       <c r="M28" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="N28" s="50" t="s">
+      <c r="N28" s="13" t="s">
         <v>477</v>
       </c>
-      <c r="O28" s="50" t="s">
+      <c r="O28" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P28" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="S28" s="53">
+      <c r="S28" s="50">
         <v>0</v>
       </c>
-      <c r="T28" s="53">
+      <c r="T28" s="50">
         <v>1</v>
       </c>
       <c r="U28" s="13">
@@ -13809,10 +13952,10 @@
       <c r="M29" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="N29" s="50" t="s">
+      <c r="N29" s="13" t="s">
         <v>478</v>
       </c>
-      <c r="O29" s="50" t="s">
+      <c r="O29" s="13" t="s">
         <v>486</v>
       </c>
       <c r="P29" s="11" t="s">
@@ -13821,7 +13964,7 @@
       <c r="Q29" s="13">
         <v>0.64</v>
       </c>
-      <c r="R29" s="53" t="s">
+      <c r="R29" s="50" t="s">
         <v>498</v>
       </c>
       <c r="U29" s="13" t="s">
@@ -13868,10 +14011,10 @@
       <c r="M30" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="N30" s="50" t="s">
+      <c r="N30" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="O30" s="50" t="s">
+      <c r="O30" s="13" t="s">
         <v>486</v>
       </c>
       <c r="P30" s="11" t="s">
@@ -13880,7 +14023,7 @@
       <c r="Q30" s="13">
         <v>0.41</v>
       </c>
-      <c r="R30" s="53" t="s">
+      <c r="R30" s="50" t="s">
         <v>498</v>
       </c>
       <c r="U30" s="13" t="s">
@@ -13927,16 +14070,16 @@
       <c r="M31" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="N31" s="50">
+      <c r="N31" s="13">
         <v>-60</v>
       </c>
-      <c r="O31" s="50" t="s">
+      <c r="O31" s="13" t="s">
         <v>487</v>
       </c>
       <c r="P31" s="11" t="s">
         <v>497</v>
       </c>
-      <c r="Q31" s="53">
+      <c r="Q31" s="50">
         <v>0.6</v>
       </c>
       <c r="U31" s="13">
@@ -13983,16 +14126,16 @@
       <c r="M32" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="N32" s="50">
+      <c r="N32" s="13">
         <v>-14.1</v>
       </c>
-      <c r="O32" s="50" t="s">
+      <c r="O32" s="13" t="s">
         <v>487</v>
       </c>
       <c r="P32" s="11" t="s">
         <v>497</v>
       </c>
-      <c r="Q32" s="53">
+      <c r="Q32" s="50">
         <v>0.14699999999999999</v>
       </c>
       <c r="U32" s="13">
@@ -14039,19 +14182,19 @@
       <c r="M33" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="N33" s="50" t="s">
+      <c r="N33" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="O33" s="50" t="s">
+      <c r="O33" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P33" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S33" s="53">
+      <c r="S33" s="50">
         <v>90</v>
       </c>
-      <c r="T33" s="53">
+      <c r="T33" s="50">
         <v>100</v>
       </c>
       <c r="U33" s="13">
@@ -14098,19 +14241,19 @@
       <c r="M34" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="N34" s="50" t="s">
+      <c r="N34" s="13" t="s">
         <v>481</v>
       </c>
-      <c r="O34" s="50" t="s">
+      <c r="O34" s="13" t="s">
         <v>20</v>
       </c>
       <c r="P34" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S34" s="53">
+      <c r="S34" s="50">
         <v>90</v>
       </c>
-      <c r="T34" s="53">
+      <c r="T34" s="50">
         <v>100</v>
       </c>
       <c r="U34" s="13">
@@ -14157,19 +14300,19 @@
       <c r="M35" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="N35" s="50">
+      <c r="N35" s="13">
         <v>28</v>
       </c>
-      <c r="O35" s="50" t="s">
+      <c r="O35" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P35" t="s">
         <v>327</v>
       </c>
-      <c r="S35" s="53">
+      <c r="S35" s="50">
         <v>50</v>
       </c>
-      <c r="T35" s="53">
+      <c r="T35" s="50">
         <v>100</v>
       </c>
       <c r="U35" s="13">
@@ -14216,19 +14359,19 @@
       <c r="M36" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="N36" s="50">
+      <c r="N36" s="13">
         <v>0</v>
       </c>
-      <c r="O36" s="50" t="s">
+      <c r="O36" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P36" t="s">
         <v>327</v>
       </c>
-      <c r="S36" s="53">
+      <c r="S36" s="50">
         <v>11</v>
       </c>
-      <c r="T36" s="53">
+      <c r="T36" s="50">
         <v>50</v>
       </c>
       <c r="U36" s="13">
@@ -14275,19 +14418,19 @@
       <c r="M37" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="N37" s="50">
+      <c r="N37" s="13">
         <v>3</v>
       </c>
-      <c r="O37" s="50" t="s">
+      <c r="O37" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P37" t="s">
         <v>327</v>
       </c>
-      <c r="S37" s="53">
+      <c r="S37" s="50">
         <v>0</v>
       </c>
-      <c r="T37" s="53">
+      <c r="T37" s="50">
         <v>10</v>
       </c>
       <c r="U37" s="13">
@@ -14334,19 +14477,19 @@
       <c r="M38" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="N38" s="50">
+      <c r="N38" s="13">
         <v>4</v>
       </c>
-      <c r="O38" s="50" t="s">
+      <c r="O38" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P38" t="s">
         <v>327</v>
       </c>
-      <c r="S38" s="53">
+      <c r="S38" s="50">
         <v>50</v>
       </c>
-      <c r="T38" s="53">
+      <c r="T38" s="50">
         <v>100</v>
       </c>
       <c r="U38" s="13">
@@ -14393,19 +14536,19 @@
       <c r="M39" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="N39" s="50">
+      <c r="N39" s="13">
         <v>2</v>
       </c>
-      <c r="O39" s="50" t="s">
+      <c r="O39" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P39" t="s">
         <v>327</v>
       </c>
-      <c r="S39" s="53">
+      <c r="S39" s="50">
         <v>11</v>
       </c>
-      <c r="T39" s="53">
+      <c r="T39" s="50">
         <v>50</v>
       </c>
       <c r="U39" s="13">
@@ -14452,19 +14595,19 @@
       <c r="M40" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="N40" s="50">
+      <c r="N40" s="13">
         <v>6</v>
       </c>
-      <c r="O40" s="50" t="s">
+      <c r="O40" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P40" t="s">
         <v>327</v>
       </c>
-      <c r="S40" s="53">
+      <c r="S40" s="50">
         <v>0</v>
       </c>
-      <c r="T40" s="53">
+      <c r="T40" s="50">
         <v>10</v>
       </c>
       <c r="U40" s="13">
@@ -14511,10 +14654,10 @@
       <c r="M41" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="N41" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="O41" s="50" t="s">
+      <c r="N41" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O41" s="13" t="s">
         <v>52</v>
       </c>
       <c r="P41" t="s">
@@ -14564,10 +14707,10 @@
       <c r="M42" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="N42" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="O42" s="50" t="s">
+      <c r="N42" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O42" s="13" t="s">
         <v>52</v>
       </c>
       <c r="P42" t="s">
@@ -14619,19 +14762,19 @@
       <c r="M43" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="N43" s="50">
+      <c r="N43" s="13">
         <v>1</v>
       </c>
-      <c r="O43" s="50" t="s">
+      <c r="O43" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P43" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S43" s="53">
+      <c r="S43" s="50">
         <v>90</v>
       </c>
-      <c r="T43" s="53">
+      <c r="T43" s="50">
         <v>100</v>
       </c>
       <c r="U43" s="13">
@@ -14680,19 +14823,19 @@
       <c r="M44" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="N44" s="50">
+      <c r="N44" s="13">
         <v>5</v>
       </c>
-      <c r="O44" s="50" t="s">
+      <c r="O44" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P44" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S44" s="53">
+      <c r="S44" s="50">
         <v>75</v>
       </c>
-      <c r="T44" s="53">
+      <c r="T44" s="50">
         <v>90</v>
       </c>
       <c r="U44" s="13">
@@ -14741,19 +14884,19 @@
       <c r="M45" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="N45" s="50">
+      <c r="N45" s="13">
         <v>2</v>
       </c>
-      <c r="O45" s="50" t="s">
+      <c r="O45" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P45" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S45" s="53">
+      <c r="S45" s="50">
         <v>50</v>
       </c>
-      <c r="T45" s="53">
+      <c r="T45" s="50">
         <v>75</v>
       </c>
       <c r="U45" s="13">
@@ -14802,19 +14945,19 @@
       <c r="M46" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="N46" s="50">
+      <c r="N46" s="13">
         <v>2</v>
       </c>
-      <c r="O46" s="50" t="s">
+      <c r="O46" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P46" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S46" s="53">
+      <c r="S46" s="50">
         <v>90</v>
       </c>
-      <c r="T46" s="53">
+      <c r="T46" s="50">
         <v>100</v>
       </c>
       <c r="U46" s="13">
@@ -14863,19 +15006,19 @@
       <c r="M47" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="N47" s="50">
+      <c r="N47" s="13">
         <v>4</v>
       </c>
-      <c r="O47" s="50" t="s">
+      <c r="O47" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P47" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S47" s="53">
+      <c r="S47" s="50">
         <v>75</v>
       </c>
-      <c r="T47" s="53">
+      <c r="T47" s="50">
         <v>90</v>
       </c>
       <c r="U47" s="13">
@@ -14924,19 +15067,19 @@
       <c r="M48" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="N48" s="50">
+      <c r="N48" s="13">
         <v>3</v>
       </c>
-      <c r="O48" s="50" t="s">
+      <c r="O48" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P48" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S48" s="53">
+      <c r="S48" s="50">
         <v>50</v>
       </c>
-      <c r="T48" s="53">
+      <c r="T48" s="50">
         <v>75</v>
       </c>
       <c r="U48" s="13">
@@ -14985,19 +15128,19 @@
       <c r="M49" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="N49" s="50">
+      <c r="N49" s="13">
         <v>1</v>
       </c>
-      <c r="O49" s="50" t="s">
+      <c r="O49" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P49" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S49" s="53">
+      <c r="S49" s="50">
         <v>0</v>
       </c>
-      <c r="T49" s="53">
+      <c r="T49" s="50">
         <v>25</v>
       </c>
       <c r="U49" s="13">
@@ -15046,19 +15189,19 @@
       <c r="M50" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="N50" s="50">
+      <c r="N50" s="13">
         <v>61.5</v>
       </c>
-      <c r="O50" s="50" t="s">
+      <c r="O50" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P50" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S50" s="53">
+      <c r="S50" s="50">
         <v>50</v>
       </c>
-      <c r="T50" s="53">
+      <c r="T50" s="50">
         <v>100</v>
       </c>
       <c r="U50" s="13">
@@ -15107,19 +15250,19 @@
       <c r="M51" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="N51" s="50">
+      <c r="N51" s="13">
         <v>30.8</v>
       </c>
-      <c r="O51" s="50" t="s">
+      <c r="O51" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P51" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S51" s="53">
+      <c r="S51" s="50">
         <v>1</v>
       </c>
-      <c r="T51" s="53">
+      <c r="T51" s="50">
         <v>50</v>
       </c>
       <c r="U51" s="13">
@@ -15168,15 +15311,13 @@
       <c r="M52" s="11" t="s">
         <v>510</v>
       </c>
-      <c r="N52" s="50"/>
-      <c r="O52" s="50"/>
       <c r="P52" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S52" s="53">
+      <c r="S52" s="50">
         <v>0</v>
       </c>
-      <c r="T52" s="53">
+      <c r="T52" s="50">
         <v>1</v>
       </c>
       <c r="U52" s="13">
@@ -15222,19 +15363,19 @@
       <c r="M53" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="N53" s="50">
+      <c r="N53" s="13">
         <v>0</v>
       </c>
-      <c r="O53" s="50" t="s">
+      <c r="O53" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P53" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S53" s="53">
+      <c r="S53" s="50">
         <v>50</v>
       </c>
-      <c r="T53" s="53">
+      <c r="T53" s="50">
         <v>100</v>
       </c>
       <c r="U53" s="13">
@@ -15283,19 +15424,19 @@
       <c r="M54" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="N54" s="50">
+      <c r="N54" s="13">
         <v>10</v>
       </c>
-      <c r="O54" s="50" t="s">
+      <c r="O54" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P54" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S54" s="53">
+      <c r="S54" s="50">
         <v>1</v>
       </c>
-      <c r="T54" s="53">
+      <c r="T54" s="50">
         <v>50</v>
       </c>
       <c r="U54" s="13">
@@ -15344,15 +15485,13 @@
       <c r="M55" s="11" t="s">
         <v>510</v>
       </c>
-      <c r="N55" s="50"/>
-      <c r="O55" s="50"/>
       <c r="P55" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S55" s="53">
+      <c r="S55" s="50">
         <v>0</v>
       </c>
-      <c r="T55" s="53">
+      <c r="T55" s="50">
         <v>1</v>
       </c>
       <c r="U55" s="13">
@@ -15398,10 +15537,10 @@
       <c r="M56" s="11" t="s">
         <v>489</v>
       </c>
-      <c r="N56" s="50">
+      <c r="N56" s="13">
         <v>44.82</v>
       </c>
-      <c r="O56" s="50" t="s">
+      <c r="O56" s="13" t="s">
         <v>330</v>
       </c>
       <c r="P56" s="11" t="s">
@@ -15410,7 +15549,7 @@
       <c r="Q56" s="13">
         <v>44.82</v>
       </c>
-      <c r="R56" s="53">
+      <c r="R56" s="50">
         <v>12.21</v>
       </c>
       <c r="U56" s="13" t="s">
@@ -15459,10 +15598,10 @@
       <c r="M57" s="11" t="s">
         <v>489</v>
       </c>
-      <c r="N57" s="50">
+      <c r="N57" s="13">
         <v>78.73</v>
       </c>
-      <c r="O57" s="50" t="s">
+      <c r="O57" s="13" t="s">
         <v>330</v>
       </c>
       <c r="P57" s="11" t="s">
@@ -15471,7 +15610,7 @@
       <c r="Q57" s="13">
         <v>78.73</v>
       </c>
-      <c r="R57" s="53">
+      <c r="R57" s="50">
         <v>22.47</v>
       </c>
       <c r="U57" s="13" t="s">
@@ -15520,19 +15659,19 @@
       <c r="M58" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="N58" s="50">
+      <c r="N58" s="13">
         <v>56</v>
       </c>
-      <c r="O58" s="50" t="s">
+      <c r="O58" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P58" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S58" s="53">
+      <c r="S58" s="50">
         <v>75</v>
       </c>
-      <c r="T58" s="53">
+      <c r="T58" s="50">
         <v>100</v>
       </c>
       <c r="U58" s="13">
@@ -15581,19 +15720,19 @@
       <c r="M59" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="N59" s="50">
+      <c r="N59" s="13">
         <v>12</v>
       </c>
-      <c r="O59" s="50" t="s">
+      <c r="O59" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P59" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S59" s="53">
+      <c r="S59" s="50">
         <v>0</v>
       </c>
-      <c r="T59" s="53">
+      <c r="T59" s="50">
         <v>75</v>
       </c>
       <c r="U59" s="13">
@@ -15642,19 +15781,19 @@
       <c r="M60" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="N60" s="50">
+      <c r="N60" s="13">
         <v>12</v>
       </c>
-      <c r="O60" s="50" t="s">
+      <c r="O60" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P60" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S60" s="53">
+      <c r="S60" s="50">
         <v>75</v>
       </c>
-      <c r="T60" s="53">
+      <c r="T60" s="50">
         <v>100</v>
       </c>
       <c r="U60" s="13">
@@ -15703,19 +15842,19 @@
       <c r="M61" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="N61" s="50">
+      <c r="N61" s="13">
         <v>30</v>
       </c>
-      <c r="O61" s="50" t="s">
+      <c r="O61" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P61" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S61" s="53">
+      <c r="S61" s="50">
         <v>0</v>
       </c>
-      <c r="T61" s="53">
+      <c r="T61" s="50">
         <v>75</v>
       </c>
       <c r="U61" s="13">
@@ -15764,19 +15903,19 @@
       <c r="M62" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="N62" s="50">
+      <c r="N62" s="13">
         <v>7.9</v>
       </c>
-      <c r="O62" s="50" t="s">
+      <c r="O62" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P62" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S62" s="53">
+      <c r="S62" s="50">
         <v>0</v>
       </c>
-      <c r="T62" s="53">
+      <c r="T62" s="50">
         <v>1</v>
       </c>
       <c r="U62" s="13">
@@ -15826,19 +15965,19 @@
       <c r="M63" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="N63" s="50">
+      <c r="N63" s="13">
         <v>35.6</v>
       </c>
-      <c r="O63" s="50" t="s">
+      <c r="O63" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P63" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S63" s="53">
+      <c r="S63" s="50">
         <v>0</v>
       </c>
-      <c r="T63" s="53">
+      <c r="T63" s="50">
         <v>1</v>
       </c>
       <c r="U63" s="13">
@@ -15888,19 +16027,19 @@
       <c r="M64" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="N64" s="50">
+      <c r="N64" s="13">
         <v>56.4</v>
       </c>
-      <c r="O64" s="50" t="s">
+      <c r="O64" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P64" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S64" s="53">
+      <c r="S64" s="50">
         <v>1</v>
       </c>
-      <c r="T64" s="53">
+      <c r="T64" s="50">
         <v>99</v>
       </c>
       <c r="U64" s="13">
@@ -15950,19 +16089,19 @@
       <c r="M65" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="N65" s="50">
+      <c r="N65" s="13">
         <v>12</v>
       </c>
-      <c r="O65" s="50" t="s">
+      <c r="O65" s="13" t="s">
         <v>319</v>
       </c>
       <c r="P65" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S65" s="53">
+      <c r="S65" s="50">
         <v>99</v>
       </c>
-      <c r="T65" s="53">
+      <c r="T65" s="50">
         <v>100</v>
       </c>
       <c r="U65" s="13">
@@ -16011,19 +16150,19 @@
       <c r="M66" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="N66" s="50">
+      <c r="N66" s="13">
         <v>65.2</v>
       </c>
-      <c r="O66" s="50" t="s">
+      <c r="O66" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P66" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S66" s="53">
+      <c r="S66" s="50">
         <v>0</v>
       </c>
-      <c r="T66" s="53">
+      <c r="T66" s="50">
         <v>1</v>
       </c>
       <c r="U66" s="13">
@@ -16073,19 +16212,19 @@
       <c r="M67" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="N67" s="50">
+      <c r="N67" s="13">
         <v>30.4</v>
       </c>
-      <c r="O67" s="50" t="s">
+      <c r="O67" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P67" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S67" s="53">
+      <c r="S67" s="50">
         <v>0</v>
       </c>
-      <c r="T67" s="53">
+      <c r="T67" s="50">
         <v>1</v>
       </c>
       <c r="U67" s="13">
@@ -16135,19 +16274,19 @@
       <c r="M68" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="N68" s="50">
+      <c r="N68" s="13">
         <v>4.3</v>
       </c>
-      <c r="O68" s="50" t="s">
+      <c r="O68" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P68" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S68" s="53">
+      <c r="S68" s="50">
         <v>1</v>
       </c>
-      <c r="T68" s="53">
+      <c r="T68" s="50">
         <v>99</v>
       </c>
       <c r="U68" s="13">
@@ -16196,10 +16335,10 @@
       <c r="M69" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="N69" s="50" t="s">
+      <c r="N69" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="O69" s="50" t="s">
+      <c r="O69" s="13" t="s">
         <v>488</v>
       </c>
       <c r="U69" s="13" t="s">
@@ -16248,19 +16387,19 @@
       <c r="M70" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="N70" s="50">
+      <c r="N70" s="13">
         <v>42</v>
       </c>
-      <c r="O70" s="50" t="s">
+      <c r="O70" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P70" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="S70" s="53">
+      <c r="S70" s="50">
         <v>99</v>
       </c>
-      <c r="T70" s="53">
+      <c r="T70" s="50">
         <v>100</v>
       </c>
       <c r="U70" s="13">
@@ -16309,19 +16448,19 @@
       <c r="M71" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="N71" s="50">
+      <c r="N71" s="13">
         <v>25</v>
       </c>
-      <c r="O71" s="50" t="s">
+      <c r="O71" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P71" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S71" s="53">
+      <c r="S71" s="50">
         <v>50</v>
       </c>
-      <c r="T71" s="53">
+      <c r="T71" s="50">
         <v>99</v>
       </c>
       <c r="U71" s="13">
@@ -16370,19 +16509,19 @@
       <c r="M72" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="N72" s="50">
+      <c r="N72" s="13">
         <v>17</v>
       </c>
-      <c r="O72" s="50" t="s">
+      <c r="O72" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P72" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S72" s="53">
+      <c r="S72" s="50">
         <v>0</v>
       </c>
-      <c r="T72" s="53">
+      <c r="T72" s="50">
         <v>50</v>
       </c>
       <c r="U72" s="13">
@@ -16431,10 +16570,10 @@
       <c r="M73" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="N73" s="50">
+      <c r="N73" s="13">
         <v>17</v>
       </c>
-      <c r="O73" s="50" t="s">
+      <c r="O73" s="13" t="s">
         <v>205</v>
       </c>
       <c r="U73" s="13">
@@ -16483,10 +16622,10 @@
       <c r="M74" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="N74" s="50">
+      <c r="N74" s="13">
         <v>4</v>
       </c>
-      <c r="O74" s="50" t="s">
+      <c r="O74" s="13" t="s">
         <v>319</v>
       </c>
       <c r="U74" s="13">
@@ -16535,10 +16674,10 @@
       <c r="M75" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="N75" s="50" t="s">
+      <c r="N75" s="13" t="s">
         <v>483</v>
       </c>
-      <c r="O75" s="50" t="s">
+      <c r="O75" s="13" t="s">
         <v>488</v>
       </c>
       <c r="U75" s="13" t="s">
@@ -16587,19 +16726,19 @@
       <c r="M76" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="N76" s="50">
+      <c r="N76" s="13">
         <v>40</v>
       </c>
-      <c r="O76" s="50" t="s">
+      <c r="O76" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P76" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S76" s="53">
+      <c r="S76" s="50">
         <v>99</v>
       </c>
-      <c r="T76" s="53">
+      <c r="T76" s="50">
         <v>100</v>
       </c>
       <c r="U76" s="13">
@@ -16648,19 +16787,19 @@
       <c r="M77" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="N77" s="50">
+      <c r="N77" s="13">
         <v>20</v>
       </c>
-      <c r="O77" s="50" t="s">
+      <c r="O77" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P77" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S77" s="53">
+      <c r="S77" s="50">
         <v>50</v>
       </c>
-      <c r="T77" s="53">
+      <c r="T77" s="50">
         <v>99</v>
       </c>
       <c r="U77" s="13">
@@ -16709,19 +16848,19 @@
       <c r="M78" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="N78" s="50">
+      <c r="N78" s="13">
         <v>20</v>
       </c>
-      <c r="O78" s="50" t="s">
+      <c r="O78" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P78" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S78" s="53">
+      <c r="S78" s="50">
         <v>0</v>
       </c>
-      <c r="T78" s="53">
+      <c r="T78" s="50">
         <v>50</v>
       </c>
       <c r="U78" s="13">
@@ -16770,19 +16909,19 @@
       <c r="M79" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="N79" s="50">
+      <c r="N79" s="13">
         <v>20</v>
       </c>
-      <c r="O79" s="50" t="s">
+      <c r="O79" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P79" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="S79" s="53">
+      <c r="S79" s="50">
         <v>0</v>
       </c>
-      <c r="T79" s="53">
+      <c r="T79" s="50">
         <v>0</v>
       </c>
       <c r="U79" s="13">
@@ -16831,10 +16970,10 @@
       <c r="M80" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="N80" s="50">
+      <c r="N80" s="13">
         <v>3</v>
       </c>
-      <c r="O80" s="50" t="s">
+      <c r="O80" s="13" t="s">
         <v>319</v>
       </c>
       <c r="U80" s="13">
@@ -16881,10 +17020,10 @@
       <c r="M81" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="N81" s="50" t="s">
+      <c r="N81" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="O81" s="50" t="s">
+      <c r="O81" s="13" t="s">
         <v>488</v>
       </c>
       <c r="P81" s="11" t="s">
@@ -16940,10 +17079,10 @@
       <c r="M82" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="N82" s="50" t="s">
+      <c r="N82" s="13" t="s">
         <v>485</v>
       </c>
-      <c r="O82" s="50" t="s">
+      <c r="O82" s="13" t="s">
         <v>488</v>
       </c>
       <c r="P82" s="11" t="s">
@@ -16999,10 +17138,10 @@
       <c r="M83" s="11" t="s">
         <v>511</v>
       </c>
-      <c r="N83" s="54" t="s">
+      <c r="N83" s="16" t="s">
         <v>504</v>
       </c>
-      <c r="O83" s="54" t="s">
+      <c r="O83" s="16" t="s">
         <v>503</v>
       </c>
       <c r="P83" s="13" t="s">
@@ -17062,10 +17201,10 @@
       <c r="M84" s="11" t="s">
         <v>507</v>
       </c>
-      <c r="N84" s="50" t="s">
+      <c r="N84" s="13" t="s">
         <v>508</v>
       </c>
-      <c r="O84" s="50" t="s">
+      <c r="O84" s="13" t="s">
         <v>503</v>
       </c>
       <c r="P84" s="13" t="s">
@@ -17089,6 +17228,1228 @@
       </c>
       <c r="W84" s="11" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B85" s="51">
+        <v>3875</v>
+      </c>
+      <c r="C85" s="52">
+        <v>23301692</v>
+      </c>
+      <c r="D85" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="F85" s="11">
+        <v>2013</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H85" s="38" t="s">
+        <v>514</v>
+      </c>
+      <c r="I85" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="J85" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="K85" s="11">
+        <v>7</v>
+      </c>
+      <c r="L85" s="11">
+        <v>6</v>
+      </c>
+      <c r="M85" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="N85" s="50" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q85" s="50">
+        <v>44.9</v>
+      </c>
+      <c r="R85" s="11"/>
+      <c r="U85" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="V85" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="W85" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B86" s="51">
+        <v>3875</v>
+      </c>
+      <c r="C86" s="52">
+        <v>23301692</v>
+      </c>
+      <c r="D86" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="F86" s="11">
+        <v>2013</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H86" s="38" t="s">
+        <v>514</v>
+      </c>
+      <c r="I86" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="J86" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="K86" s="11">
+        <v>7</v>
+      </c>
+      <c r="L86" s="11">
+        <v>6</v>
+      </c>
+      <c r="M86" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="N86" s="50" t="s">
+        <v>547</v>
+      </c>
+      <c r="Q86" s="50">
+        <v>15.8</v>
+      </c>
+      <c r="R86" s="11"/>
+      <c r="U86" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="V86" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="W86" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B87" s="51">
+        <v>3875</v>
+      </c>
+      <c r="C87" s="52">
+        <v>23301692</v>
+      </c>
+      <c r="D87" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="F87" s="11">
+        <v>2013</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H87" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I87" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J87" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K87" s="11">
+        <v>7</v>
+      </c>
+      <c r="L87" s="11">
+        <v>6</v>
+      </c>
+      <c r="M87" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="N87" s="50">
+        <v>-11.3</v>
+      </c>
+      <c r="Q87" s="50">
+        <v>-11.3</v>
+      </c>
+      <c r="R87" s="11"/>
+      <c r="U87" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="V87" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="W87" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B88" s="51">
+        <v>3875</v>
+      </c>
+      <c r="C88" s="52">
+        <v>23301692</v>
+      </c>
+      <c r="D88" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="F88" s="11">
+        <v>2013</v>
+      </c>
+      <c r="G88" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H88" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I88" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J88" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K88" s="11">
+        <v>7</v>
+      </c>
+      <c r="L88" s="11">
+        <v>6</v>
+      </c>
+      <c r="M88" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="N88" s="50">
+        <v>-8.9</v>
+      </c>
+      <c r="Q88" s="50">
+        <v>-8.9</v>
+      </c>
+      <c r="R88" s="11"/>
+      <c r="U88" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="V88" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="W88" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B89" s="51">
+        <v>3843</v>
+      </c>
+      <c r="C89" s="52">
+        <v>23301692</v>
+      </c>
+      <c r="D89" s="53" t="s">
+        <v>515</v>
+      </c>
+      <c r="E89" s="54" t="s">
+        <v>516</v>
+      </c>
+      <c r="F89" s="11">
+        <v>2013</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H89" s="36" t="s">
+        <v>517</v>
+      </c>
+      <c r="I89" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="J89" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="K89" s="11">
+        <v>10</v>
+      </c>
+      <c r="L89" s="11">
+        <v>5</v>
+      </c>
+      <c r="M89" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="R89" s="11">
+        <v>1.7</v>
+      </c>
+      <c r="U89" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="V89" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="W89" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B90" s="51">
+        <v>3843</v>
+      </c>
+      <c r="C90" s="52">
+        <v>24314186</v>
+      </c>
+      <c r="D90" s="53" t="s">
+        <v>515</v>
+      </c>
+      <c r="E90" s="54" t="s">
+        <v>516</v>
+      </c>
+      <c r="F90" s="11">
+        <v>2013</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="H90" s="25" t="s">
+        <v>518</v>
+      </c>
+      <c r="I90" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="J90" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="K90" s="11">
+        <v>10</v>
+      </c>
+      <c r="L90" s="11">
+        <v>4</v>
+      </c>
+      <c r="M90" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="R90" s="11">
+        <v>2.9</v>
+      </c>
+      <c r="U90" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="V90" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="W90" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B91" s="51">
+        <v>3843</v>
+      </c>
+      <c r="C91" s="52">
+        <v>24314186</v>
+      </c>
+      <c r="D91" s="53" t="s">
+        <v>515</v>
+      </c>
+      <c r="E91" s="54" t="s">
+        <v>516</v>
+      </c>
+      <c r="F91" s="11">
+        <v>2013</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H91" s="36" t="s">
+        <v>517</v>
+      </c>
+      <c r="I91" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="J91" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="K91" s="11">
+        <v>10</v>
+      </c>
+      <c r="L91" s="11">
+        <v>5</v>
+      </c>
+      <c r="M91" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="N91" s="13" t="s">
+        <v>548</v>
+      </c>
+      <c r="Q91" s="50">
+        <v>89.8</v>
+      </c>
+      <c r="R91" s="11">
+        <v>10.3</v>
+      </c>
+      <c r="U91" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="V91" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="W91" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B92" s="51">
+        <v>3843</v>
+      </c>
+      <c r="C92" s="52">
+        <v>24314186</v>
+      </c>
+      <c r="D92" s="53" t="s">
+        <v>515</v>
+      </c>
+      <c r="E92" s="54" t="s">
+        <v>516</v>
+      </c>
+      <c r="F92" s="11">
+        <v>2013</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="H92" s="25" t="s">
+        <v>518</v>
+      </c>
+      <c r="I92" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="J92" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="K92" s="11">
+        <v>10</v>
+      </c>
+      <c r="L92" s="11">
+        <v>4</v>
+      </c>
+      <c r="M92" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="N92" s="13" t="s">
+        <v>549</v>
+      </c>
+      <c r="Q92" s="50">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="R92" s="11">
+        <v>41.6</v>
+      </c>
+      <c r="U92" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="V92" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="W92" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B93" s="51">
+        <v>4000</v>
+      </c>
+      <c r="C93" s="55"/>
+      <c r="D93" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="F93" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G93" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H93" s="17">
+        <v>5</v>
+      </c>
+      <c r="I93" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="J93" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K93" s="11">
+        <v>30</v>
+      </c>
+      <c r="L93" s="11">
+        <v>30</v>
+      </c>
+      <c r="M93" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="R93" s="13"/>
+      <c r="U93" s="13">
+        <v>0</v>
+      </c>
+      <c r="V93" s="13">
+        <v>0</v>
+      </c>
+      <c r="W93" s="11" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B94" s="51">
+        <v>4000</v>
+      </c>
+      <c r="C94" s="55"/>
+      <c r="D94" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="F94" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G94" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H94" s="17">
+        <v>5</v>
+      </c>
+      <c r="I94" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="J94" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K94" s="11">
+        <v>30</v>
+      </c>
+      <c r="L94" s="11">
+        <v>30</v>
+      </c>
+      <c r="M94" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="R94" s="13"/>
+      <c r="U94" s="13">
+        <v>1</v>
+      </c>
+      <c r="V94" s="13">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B95" s="51">
+        <v>4000</v>
+      </c>
+      <c r="C95" s="55"/>
+      <c r="D95" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="F95" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G95" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H95" s="17">
+        <v>5</v>
+      </c>
+      <c r="I95" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="J95" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K95" s="11">
+        <v>30</v>
+      </c>
+      <c r="L95" s="11">
+        <v>30</v>
+      </c>
+      <c r="M95" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="R95" s="13"/>
+      <c r="U95" s="13">
+        <v>1</v>
+      </c>
+      <c r="V95" s="13">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B96" s="51">
+        <v>4000</v>
+      </c>
+      <c r="C96" s="55"/>
+      <c r="D96" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="F96" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G96" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H96" s="17">
+        <v>5</v>
+      </c>
+      <c r="I96" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="J96" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K96" s="11">
+        <v>30</v>
+      </c>
+      <c r="L96" s="11">
+        <v>30</v>
+      </c>
+      <c r="M96" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="R96" s="13"/>
+      <c r="U96" s="13">
+        <v>3</v>
+      </c>
+      <c r="V96" s="13">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B97" s="51">
+        <v>4000</v>
+      </c>
+      <c r="C97" s="55"/>
+      <c r="D97" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="F97" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G97" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H97" s="17">
+        <v>5</v>
+      </c>
+      <c r="I97" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="J97" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K97" s="11">
+        <v>30</v>
+      </c>
+      <c r="L97" s="11">
+        <v>30</v>
+      </c>
+      <c r="M97" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="R97" s="13"/>
+      <c r="U97" s="13">
+        <v>3</v>
+      </c>
+      <c r="V97" s="13">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B98" s="51">
+        <v>4000</v>
+      </c>
+      <c r="C98" s="55"/>
+      <c r="D98" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="F98" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G98" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H98" s="17">
+        <v>5</v>
+      </c>
+      <c r="I98" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="J98" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K98" s="11">
+        <v>30</v>
+      </c>
+      <c r="L98" s="11">
+        <v>30</v>
+      </c>
+      <c r="M98" s="11" t="s">
+        <v>532</v>
+      </c>
+      <c r="R98" s="13"/>
+      <c r="U98" s="13">
+        <v>4</v>
+      </c>
+      <c r="V98" s="13">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B99" s="51">
+        <v>4000</v>
+      </c>
+      <c r="C99" s="55"/>
+      <c r="D99" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="F99" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G99" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H99" s="17">
+        <v>5</v>
+      </c>
+      <c r="I99" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="J99" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K99" s="11">
+        <v>30</v>
+      </c>
+      <c r="L99" s="11">
+        <v>30</v>
+      </c>
+      <c r="M99" s="11" t="s">
+        <v>533</v>
+      </c>
+      <c r="R99" s="13"/>
+      <c r="U99" s="13">
+        <v>3</v>
+      </c>
+      <c r="V99" s="13">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B100" s="51">
+        <v>4000</v>
+      </c>
+      <c r="C100" s="55"/>
+      <c r="D100" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="F100" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G100" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H100" s="17">
+        <v>5</v>
+      </c>
+      <c r="I100" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="J100" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K100" s="11">
+        <v>30</v>
+      </c>
+      <c r="L100" s="11">
+        <v>30</v>
+      </c>
+      <c r="M100" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="R100" s="13"/>
+      <c r="U100" s="13">
+        <v>3</v>
+      </c>
+      <c r="V100" s="13">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B101" s="51">
+        <v>4000</v>
+      </c>
+      <c r="C101" s="55"/>
+      <c r="D101" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="F101" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G101" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H101" s="17">
+        <v>5</v>
+      </c>
+      <c r="I101" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="J101" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K101" s="11">
+        <v>30</v>
+      </c>
+      <c r="L101" s="11">
+        <v>30</v>
+      </c>
+      <c r="M101" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="R101" s="13"/>
+      <c r="U101" s="13">
+        <v>6</v>
+      </c>
+      <c r="V101" s="13">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B102" s="51">
+        <v>4000</v>
+      </c>
+      <c r="C102" s="55"/>
+      <c r="D102" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="F102" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G102" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H102" s="17">
+        <v>5</v>
+      </c>
+      <c r="I102" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="J102" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K102" s="11">
+        <v>30</v>
+      </c>
+      <c r="L102" s="11">
+        <v>30</v>
+      </c>
+      <c r="M102" s="11" t="s">
+        <v>536</v>
+      </c>
+      <c r="R102" s="13"/>
+      <c r="U102" s="13">
+        <v>6</v>
+      </c>
+      <c r="V102" s="13">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B103" s="51">
+        <v>4000</v>
+      </c>
+      <c r="C103" s="55"/>
+      <c r="D103" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="F103" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G103" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H103" s="17">
+        <v>5</v>
+      </c>
+      <c r="I103" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="J103" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K103" s="11">
+        <v>30</v>
+      </c>
+      <c r="L103" s="11">
+        <v>30</v>
+      </c>
+      <c r="M103" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="R103" s="13"/>
+      <c r="U103" s="13">
+        <v>1.67</v>
+      </c>
+      <c r="V103" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B104" s="57">
+        <v>4007</v>
+      </c>
+      <c r="C104" s="17"/>
+      <c r="D104" s="58" t="s">
+        <v>521</v>
+      </c>
+      <c r="E104" s="56" t="s">
+        <v>522</v>
+      </c>
+      <c r="F104" s="56">
+        <v>2014</v>
+      </c>
+      <c r="G104" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H104" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I104" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="J104" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K104" s="11">
+        <v>61</v>
+      </c>
+      <c r="L104" s="11">
+        <v>61</v>
+      </c>
+      <c r="M104" s="11" t="s">
+        <v>538</v>
+      </c>
+      <c r="R104" s="13"/>
+      <c r="U104" s="13">
+        <v>0</v>
+      </c>
+      <c r="V104" s="13">
+        <v>0</v>
+      </c>
+      <c r="W104" s="11" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B105" s="57">
+        <v>4007</v>
+      </c>
+      <c r="C105" s="17"/>
+      <c r="D105" s="58" t="s">
+        <v>521</v>
+      </c>
+      <c r="E105" s="56" t="s">
+        <v>522</v>
+      </c>
+      <c r="F105" s="56">
+        <v>2014</v>
+      </c>
+      <c r="G105" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H105" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I105" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="J105" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K105" s="11">
+        <v>61</v>
+      </c>
+      <c r="L105" s="11">
+        <v>61</v>
+      </c>
+      <c r="M105" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="R105" s="13"/>
+      <c r="U105" s="13">
+        <v>3</v>
+      </c>
+      <c r="V105" s="13">
+        <v>4.92</v>
+      </c>
+      <c r="W105" s="11" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B106" s="57">
+        <v>4007</v>
+      </c>
+      <c r="C106" s="17"/>
+      <c r="D106" s="58" t="s">
+        <v>521</v>
+      </c>
+      <c r="E106" s="56" t="s">
+        <v>522</v>
+      </c>
+      <c r="F106" s="56">
+        <v>2014</v>
+      </c>
+      <c r="G106" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H106" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I106" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="J106" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K106" s="11">
+        <v>61</v>
+      </c>
+      <c r="L106" s="11">
+        <v>61</v>
+      </c>
+      <c r="M106" s="11" t="s">
+        <v>540</v>
+      </c>
+      <c r="R106" s="13"/>
+      <c r="U106" s="13">
+        <v>19</v>
+      </c>
+      <c r="V106" s="13">
+        <v>31.15</v>
+      </c>
+      <c r="W106" s="11" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B107" s="57">
+        <v>4007</v>
+      </c>
+      <c r="C107" s="17"/>
+      <c r="D107" s="58" t="s">
+        <v>521</v>
+      </c>
+      <c r="E107" s="56" t="s">
+        <v>522</v>
+      </c>
+      <c r="F107" s="56">
+        <v>2014</v>
+      </c>
+      <c r="G107" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H107" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I107" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="J107" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K107" s="11">
+        <v>61</v>
+      </c>
+      <c r="L107" s="11">
+        <v>61</v>
+      </c>
+      <c r="M107" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="R107" s="13"/>
+      <c r="U107" s="13">
+        <v>11</v>
+      </c>
+      <c r="V107" s="13">
+        <v>18.03</v>
+      </c>
+      <c r="W107" s="11" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B108" s="57">
+        <v>4007</v>
+      </c>
+      <c r="C108" s="17"/>
+      <c r="D108" s="58" t="s">
+        <v>521</v>
+      </c>
+      <c r="E108" s="56" t="s">
+        <v>522</v>
+      </c>
+      <c r="F108" s="56">
+        <v>2014</v>
+      </c>
+      <c r="G108" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H108" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I108" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="J108" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K108" s="11">
+        <v>61</v>
+      </c>
+      <c r="L108" s="11">
+        <v>61</v>
+      </c>
+      <c r="M108" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="R108" s="13"/>
+      <c r="U108" s="13">
+        <v>14</v>
+      </c>
+      <c r="V108" s="13">
+        <v>22.95</v>
+      </c>
+      <c r="W108" s="11" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B109" s="57">
+        <v>4007</v>
+      </c>
+      <c r="C109" s="17"/>
+      <c r="D109" s="58" t="s">
+        <v>521</v>
+      </c>
+      <c r="E109" s="56" t="s">
+        <v>522</v>
+      </c>
+      <c r="F109" s="56">
+        <v>2014</v>
+      </c>
+      <c r="G109" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H109" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I109" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="J109" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="K109" s="11">
+        <v>61</v>
+      </c>
+      <c r="L109" s="11">
+        <v>61</v>
+      </c>
+      <c r="M109" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="R109" s="13"/>
+      <c r="U109" s="13">
+        <v>14</v>
+      </c>
+      <c r="V109" s="13">
+        <v>22.95</v>
+      </c>
+      <c r="W109" s="11" t="s">
+        <v>545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>